<commit_message>
reduce % of S industrial buildings from 55% to 20% following local expert feedback
</commit_message>
<xml_diff>
--- a/ind_mapping_schemes/mapping_Romania_IND.xlsx
+++ b/ind_mapping_schemes/mapping_Romania_IND.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/ind_mapping_schemes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A4787D-7BBE-9440-8D16-07BE313BFF3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_ind" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -19,20 +25,20 @@
     <t>industrial</t>
   </si>
   <si>
-    <t>24% CR/LFM+CDM/H:1
-1% CR/LFM+CDM/H:1
-20% CR+PC/LFM+CDL/H:1
-15% S+SL/LFM+CDM/H:1
-30% S/LFM+CDM/RME/H:1
-8% S/LFBR+CDH/H:1
-2% S/LFBR+CDM/H:1</t>
+    <t>43% CR/LFM+CDM/H:1
+2% CR/LFM+CDM/H:1
+35% CR+PC/LFM+CDL/H:1
+5% S+SL/LFM+CDM/H:1
+11% S/LFM+CDM/RME/H:1
+3% S/LFBR+CDH/H:1
+1% S/LFBR+CDM/H:1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,10 +90,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -95,6 +104,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -141,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -173,9 +190,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,6 +242,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,20 +435,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
+    <row r="2" spans="2:2" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>